<commit_message>
Adapt to the Northwind sample database
</commit_message>
<xml_diff>
--- a/DbToExcel/Test.xlsx
+++ b/DbToExcel/Test.xlsx
@@ -16,33 +16,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Modality</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Component Name</t>
-  </si>
-  <si>
-    <t>Component ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Study ID</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Inspector</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact Title</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
   </si>
 </sst>
 </file>
@@ -390,23 +393,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -418,16 +430,19 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>